<commit_message>
Subida final de archivos procesados
Juro solemnemente no volver a tocar un PCAP (PCAPNG)
</commit_message>
<xml_diff>
--- a/Datasets/ICS1/Documentos generados/Script Proceso y Validación/RESULTADOS_EXCEL.xlsx
+++ b/Datasets/ICS1/Documentos generados/Script Proceso y Validación/RESULTADOS_EXCEL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1651939761.054205</v>
+        <v>1651938747.240006</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
@@ -516,20 +516,20 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>49964</v>
+        <v>49950</v>
       </c>
       <c r="I2" t="n">
         <v>20000</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>csv_T0882_DNP3-Directory-Read[2]_flows.xlsx</t>
+          <t>csv_T0831_DNP3-Rogue-Master-1-mod_fixed[2]_flows.xlsx</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -565,7 +565,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>csv_T0882_DNP3-File-Read-1[2]_flows.xlsx</t>
+          <t>csv_T0882_DNP3-File-Read-1-mod_fixed[2]_flows.xlsx</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1651941261.303657</v>
+        <v>1651941572.844525</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
@@ -607,13 +607,13 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>csv_T0882_DNP3-File-Read-2[2]_flows.xlsx</t>
+          <t>csv_T0882_DNP3-File-Write-1-mod_fixed[2]_flows.xlsx</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -621,35 +621,35 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1649260613.014702</v>
+        <v>1654429285.443855</v>
       </c>
       <c r="D5" t="n">
         <v>6</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0x0119</t>
+          <t>0x0018</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>192.168.0.142</t>
+          <t>192.168.2.91</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>192.168.0.64</t>
+          <t>192.168.2.86</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>57084</v>
+        <v>51929</v>
       </c>
       <c r="I5" t="n">
-        <v>102</v>
+        <v>20000</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>csv_T0882_Discovery-node-red-2[2]_flows.xlsx</t>
+          <t>csv_T0848_DNP3-Rogue-Master-mod_fixed[2]_flows.xlsx</t>
         </is>
       </c>
     </row>
@@ -663,41 +663,41 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1649260611.723868</v>
+        <v>1651939761.054205</v>
       </c>
       <c r="D6" t="n">
         <v>6</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0x0119</t>
+          <t>0x0018</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>192.168.0.142</t>
+          <t>192.168.2.91</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>192.168.0.64</t>
+          <t>192.168.2.86</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>57086</v>
+        <v>49964</v>
       </c>
       <c r="I6" t="n">
-        <v>102</v>
+        <v>20000</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>csv_T0882_Discovery-node-red-2[2]_flows.xlsx</t>
+          <t>csv_T0882_DNP3-Directory-Read-mod_fixed[2]_flows.xlsx</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1651941572.844525</v>
+        <v>1651941261.303657</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
@@ -733,385 +733,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>csv_T0882_DNP3-File-Write-1[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1651938747.240006</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0x0018</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>192.168.2.91</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>192.168.2.86</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>49950</v>
-      </c>
-      <c r="I8" t="n">
-        <v>20000</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>csv_T0831_DNP3-Rogue-Master-1[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1654429285.443855</v>
-      </c>
-      <c r="D9" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0x0018</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>192.168.2.91</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>192.168.2.86</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>51929</v>
-      </c>
-      <c r="I9" t="n">
-        <v>20000</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>csv_T0848_DNP3-Rogue-Master[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1649260322.573032</v>
-      </c>
-      <c r="D10" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0x0111</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>192.168.0.64</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>57032</v>
-      </c>
-      <c r="I10" t="n">
-        <v>102</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>csv_T0882_Discovery-node-red[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1649260367.072246</v>
-      </c>
-      <c r="D11" t="n">
-        <v>6</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0x0018</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>52.84.65.89</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>47432</v>
-      </c>
-      <c r="I11" t="n">
-        <v>443</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>csv_T0882_Discovery-node-red[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>5</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1649260329.353022</v>
-      </c>
-      <c r="D12" t="n">
-        <v>6</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0x0010</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>52.84.65.13</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>34258</v>
-      </c>
-      <c r="I12" t="n">
-        <v>443</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>csv_T0882_Discovery-node-red[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>6</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1649260329.353044</v>
-      </c>
-      <c r="D13" t="n">
-        <v>6</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0x0010</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>52.84.65.13</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>34254</v>
-      </c>
-      <c r="I13" t="n">
-        <v>443</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>csv_T0882_Discovery-node-red[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1649260319.629281</v>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0x0010</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>93.184.220.29</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>36834</v>
-      </c>
-      <c r="I14" t="n">
-        <v>80</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>csv_T0882_Discovery-node-red[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1649261659.782926</v>
-      </c>
-      <c r="D15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0x0119</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>192.168.0.64</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>57308</v>
-      </c>
-      <c r="I15" t="n">
-        <v>102</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>csv_T0879_node-red-escritura[2]_flows.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1649261665.162927</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0x0010</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>192.168.0.142</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>93.184.220.29</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>36838</v>
-      </c>
-      <c r="I16" t="n">
-        <v>80</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>csv_T0879_node-red-escritura[2]_flows.xlsx</t>
+          <t>csv_T0882_DNP3-File-Read-2-mod_fixed[2]_flows.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>